<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2025-11-20.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2025-11-20.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2025-11-20.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -523,10 +523,100 @@
       <c r="A11" t="str">
         <v>3</v>
       </c>
+      <c r="C11" t="str">
+        <v>556_马尾松_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F11" t="str">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" xml:space="preserve">
+      <c r="C12" t="str" xml:space="preserve">
+        <v xml:space="preserve">345_天竺少女_Cryptomeria
+Kashiwaba_undefined_1bunch</v>
+      </c>
+      <c r="F12" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>4</v>
+      </c>
+      <c r="C13" t="str">
+        <v>342_南天竹红_undefined_Nandina domestica Thunb._1bunch</v>
+      </c>
+      <c r="F13" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="str">
+        <v>343_南天竹带果_undefined_Nandina domestica Thunb._1bunch</v>
+      </c>
+      <c r="F14" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="str">
+        <v>321_雪柳叶_Spiraea  leaves_undefined_1bunch</v>
+      </c>
+      <c r="F15" t="str">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="str">
+        <v>106_绣球单瓣粉_Hydrangea Pink S_Hydrangea L._1stem</v>
+      </c>
+      <c r="F16" t="str">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="str">
+        <v>110_绣球单瓣浅蓝_Hydrangea Light Blue S_Hydrangea L._1stem</v>
+      </c>
+      <c r="F17" t="str">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="str">
+        <v>11_香槟洋桔梗_Champagne Lisianthus_Eustoma grandiflorum (Raf.) Shinners_800/600g</v>
+      </c>
+      <c r="F18" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="str">
+        <v>624_多丁白_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F19" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>5</v>
+      </c>
+      <c r="C20" t="str">
+        <v>475_诺贝松_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F20" t="str">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="str">
+        <v>597_尤加利叶小叶_undefined_undefined_1bunch</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L21"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -584,7 +674,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>01611121010161410100</v>
+        <v>016111210101614101030101010305040105200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>